<commit_message>
Updates from Council meeting
</commit_message>
<xml_diff>
--- a/print/Council Signin.xlsx
+++ b/print/Council Signin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\dfwtrainshows\print\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DC90A8-4350-46B8-92C4-9C682B3AA78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5CA5EA-D208-49AC-A23E-6DAD03B945A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FEE54A42-A726-4F37-A952-B97DF220F03B}"/>
+    <workbookView xWindow="3060" yWindow="1596" windowWidth="19212" windowHeight="9216" activeTab="1" xr2:uid="{FEE54A42-A726-4F37-A952-B97DF220F03B}"/>
   </bookViews>
   <sheets>
     <sheet name="Participants" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="100">
   <si>
     <t>SHOW SHARE COMMITMENT LIST</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>Alt</t>
+  </si>
+  <si>
+    <t>DAP</t>
+  </si>
+  <si>
+    <t>Dallas &amp; All Points MRR Club</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,6 +601,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC5CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -896,7 +908,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1177,6 +1189,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1191,34 +1227,6 @@
     </xf>
     <xf numFmtId="15" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1598,7 +1606,7 @@
             <v>Plano Fall Friday</v>
           </cell>
           <cell r="H4" t="str">
-            <v>Friday 9/xx/2024</v>
+            <v>Friday 9/27/2024</v>
           </cell>
         </row>
         <row r="5">
@@ -1606,7 +1614,7 @@
             <v>Plano Fall Saturday</v>
           </cell>
           <cell r="H5" t="str">
-            <v>Saturday 9/xx1/2025</v>
+            <v>Saturday 9/28/2024</v>
           </cell>
         </row>
         <row r="6">
@@ -1614,7 +1622,7 @@
             <v>Plano Fall Sunday</v>
           </cell>
           <cell r="H6" t="str">
-            <v>Sunday 9/xx/2025</v>
+            <v>Sunday 9/29/2024</v>
           </cell>
         </row>
         <row r="7">
@@ -1622,7 +1630,7 @@
             <v>Plano Jan Friday</v>
           </cell>
           <cell r="H7" t="str">
-            <v>Friday 01/xx/2026</v>
+            <v>Friday 01/17/2025</v>
           </cell>
         </row>
         <row r="8">
@@ -1630,7 +1638,7 @@
             <v>Plano Jan Saturday</v>
           </cell>
           <cell r="H8" t="str">
-            <v>Saturday 01/xx/2026</v>
+            <v>Saturday 01/18/2025</v>
           </cell>
         </row>
         <row r="9">
@@ -1638,7 +1646,7 @@
             <v>Plano Jan Sunday</v>
           </cell>
           <cell r="H9" t="str">
-            <v>Sunday 01/xx/2026</v>
+            <v>Sunday 01/19/2025</v>
           </cell>
         </row>
       </sheetData>
@@ -1677,7 +1685,7 @@
         </row>
         <row r="9">
           <cell r="C9">
-            <v>2</v>
+            <v>9</v>
           </cell>
           <cell r="D9" t="str">
             <v>BNRR</v>
@@ -1693,11 +1701,15 @@
         </row>
         <row r="11">
           <cell r="C11">
-            <v>2</v>
+            <v>8</v>
           </cell>
           <cell r="D11" t="str">
             <v>NTNG</v>
           </cell>
+        </row>
+        <row r="12">
+          <cell r="C12"/>
+          <cell r="D12"/>
         </row>
         <row r="13">
           <cell r="C13">
@@ -1707,6 +1719,14 @@
             <v>LM</v>
           </cell>
         </row>
+        <row r="14">
+          <cell r="C14"/>
+          <cell r="D14"/>
+        </row>
+        <row r="15">
+          <cell r="C15"/>
+          <cell r="D15"/>
+        </row>
         <row r="16">
           <cell r="C16">
             <v>8</v>
@@ -1723,6 +1743,14 @@
             <v>LSF</v>
           </cell>
         </row>
+        <row r="18">
+          <cell r="C18"/>
+          <cell r="D18"/>
+        </row>
+        <row r="19">
+          <cell r="C19"/>
+          <cell r="D19"/>
+        </row>
         <row r="20">
           <cell r="C20">
             <v>8</v>
@@ -1747,6 +1775,14 @@
             <v>TNT</v>
           </cell>
         </row>
+        <row r="23">
+          <cell r="C23"/>
+          <cell r="D23"/>
+        </row>
+        <row r="24">
+          <cell r="C24"/>
+          <cell r="D24"/>
+        </row>
         <row r="25">
           <cell r="C25">
             <v>14</v>
@@ -1771,6 +1807,10 @@
             <v>NTXG</v>
           </cell>
         </row>
+        <row r="28">
+          <cell r="C28"/>
+          <cell r="D28"/>
+        </row>
         <row r="29">
           <cell r="C29">
             <v>5</v>
@@ -1824,7 +1864,7 @@
             <v>2</v>
           </cell>
           <cell r="D35" t="str">
-            <v>SDCM</v>
+            <v>DAP</v>
           </cell>
         </row>
         <row r="36">
@@ -1843,6 +1883,10 @@
             <v>LSR</v>
           </cell>
         </row>
+        <row r="38">
+          <cell r="C38"/>
+          <cell r="D38"/>
+        </row>
         <row r="39">
           <cell r="C39">
             <v>1</v>
@@ -1859,6 +1903,10 @@
             <v>TRD</v>
           </cell>
         </row>
+        <row r="41">
+          <cell r="C41"/>
+          <cell r="D41"/>
+        </row>
         <row r="99">
           <cell r="C99" t="str">
             <v>Hours</v>
@@ -1923,6 +1971,14 @@
             <v>LM</v>
           </cell>
         </row>
+        <row r="107">
+          <cell r="C107"/>
+          <cell r="D107"/>
+        </row>
+        <row r="108">
+          <cell r="C108"/>
+          <cell r="D108"/>
+        </row>
         <row r="109">
           <cell r="C109">
             <v>8</v>
@@ -1939,6 +1995,10 @@
             <v>LSF</v>
           </cell>
         </row>
+        <row r="111">
+          <cell r="C111"/>
+          <cell r="D111"/>
+        </row>
         <row r="112">
           <cell r="C112">
             <v>8</v>
@@ -1963,6 +2023,14 @@
             <v>SC</v>
           </cell>
         </row>
+        <row r="115">
+          <cell r="C115"/>
+          <cell r="D115"/>
+        </row>
+        <row r="116">
+          <cell r="C116"/>
+          <cell r="D116"/>
+        </row>
         <row r="117">
           <cell r="C117">
             <v>1</v>
@@ -2040,7 +2108,7 @@
             <v>2</v>
           </cell>
           <cell r="D126" t="str">
-            <v>SDCM</v>
+            <v>DAP</v>
           </cell>
         </row>
         <row r="127">
@@ -2059,6 +2127,10 @@
             <v>LSR</v>
           </cell>
         </row>
+        <row r="129">
+          <cell r="C129"/>
+          <cell r="D129"/>
+        </row>
         <row r="130">
           <cell r="C130">
             <v>1</v>
@@ -2075,58 +2147,62 @@
             <v>TRD</v>
           </cell>
         </row>
+        <row r="132">
+          <cell r="C132"/>
+          <cell r="D132"/>
+        </row>
         <row r="180">
           <cell r="C180">
-            <v>743</v>
+            <v>756</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
         <row r="5">
           <cell r="A5" t="str">
-            <v>Friday 9/xx/2024</v>
+            <v>Friday 9/27/2024</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="4">
         <row r="5">
           <cell r="A5" t="str">
-            <v>Saturday 9/xx1/2025</v>
+            <v>Saturday 9/28/2024</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="5">
         <row r="5">
           <cell r="A5" t="str">
-            <v>Sunday 9/xx/2025</v>
+            <v>Sunday 9/29/2024</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="6">
         <row r="5">
           <cell r="A5" t="str">
-            <v>Friday 01/xx/2026</v>
+            <v>Friday 01/17/2025</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="7">
         <row r="5">
           <cell r="A5" t="str">
-            <v>Saturday 01/xx/2026</v>
+            <v>Saturday 01/18/2025</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="8">
         <row r="5">
           <cell r="A5" t="str">
-            <v>Sunday 01/xx/2026</v>
+            <v>Sunday 01/19/2025</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="9">
         <row r="2">
           <cell r="C2" t="str">
-            <v>SDCM</v>
+            <v>BNRR</v>
           </cell>
         </row>
       </sheetData>
@@ -2495,12 +2571,12 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="107"/>
       <c r="E2" s="9"/>
       <c r="F2" s="10"/>
       <c r="G2" s="11"/>
@@ -2510,10 +2586,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="97"/>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="107"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
       <c r="G3" s="11"/>
@@ -2564,12 +2640,12 @@
       <c r="H6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="100" t="s">
+      <c r="I6" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="109"/>
     </row>
     <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
@@ -3518,7 +3594,7 @@
       </c>
       <c r="C37" s="89">
         <f>GrandTotalHours</f>
-        <v>743</v>
+        <v>756</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="89">
@@ -3542,7 +3618,7 @@
       </c>
       <c r="C39" s="91">
         <f>GrandTotalHours/TotalShowShares</f>
-        <v>18.121951219512194</v>
+        <v>18.439024390243901</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="89"/>
@@ -3567,8 +3643,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="PrintParticipantShares">
+        <control shapeId="1025" r:id="rId4" name="PrintParticipantList">
           <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>30480</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>30480</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>1569720</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>137160</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="PrintParticipantList"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId6" name="PrintParticipantShares">
+          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
@@ -3587,32 +3688,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="PrintParticipantShares"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="PrintParticipantList">
-          <controlPr defaultSize="0" print="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>30480</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>30480</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>1569720</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>137160</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="PrintParticipantList"/>
+        <control shapeId="1026" r:id="rId6" name="PrintParticipantShares"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3629,31 +3705,31 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="39.5546875" defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" style="110" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="106" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" style="103" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" style="103" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="99" customWidth="1"/>
+    <col min="4" max="4" width="47.88671875" customWidth="1"/>
     <col min="5" max="5" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" style="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" t="s">
         <v>93</v>
       </c>
       <c r="E1" t="s">
@@ -3663,14 +3739,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="40.799999999999997" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="98" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="96"/>
@@ -3688,14 +3764,14 @@
       <c r="L2" s="39"/>
       <c r="M2" s="39"/>
     </row>
-    <row r="3" spans="1:13" ht="39.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="98" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="96"/>
@@ -3713,14 +3789,14 @@
       <c r="L3" s="39"/>
       <c r="M3" s="39"/>
     </row>
-    <row r="4" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="98" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="96"/>
@@ -3738,14 +3814,14 @@
       <c r="L4" s="39"/>
       <c r="M4" s="39"/>
     </row>
-    <row r="5" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="105" t="s">
+      <c r="C5" s="98" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="96"/>
@@ -3763,14 +3839,14 @@
       <c r="L5" s="39"/>
       <c r="M5" s="39"/>
     </row>
-    <row r="6" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="98" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="96"/>
@@ -3788,14 +3864,14 @@
       <c r="L6" s="39"/>
       <c r="M6" s="39"/>
     </row>
-    <row r="7" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="105" t="s">
+      <c r="C7" s="98" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="96"/>
@@ -3813,14 +3889,14 @@
       <c r="L7" s="39"/>
       <c r="M7" s="39"/>
     </row>
-    <row r="8" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="105" t="s">
+      <c r="C8" s="98" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="96"/>
@@ -3838,14 +3914,14 @@
       <c r="L8" s="39"/>
       <c r="M8" s="39"/>
     </row>
-    <row r="9" spans="1:13" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="98" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="96"/>
@@ -3863,14 +3939,14 @@
       <c r="L9" s="39"/>
       <c r="M9" s="39"/>
     </row>
-    <row r="10" spans="1:13" ht="38.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="98" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="96"/>
@@ -3888,14 +3964,14 @@
       <c r="L10" s="39"/>
       <c r="M10" s="39"/>
     </row>
-    <row r="11" spans="1:13" ht="41.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="98" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="96"/>
@@ -3913,14 +3989,14 @@
       <c r="L11" s="39"/>
       <c r="M11" s="39"/>
     </row>
-    <row r="12" spans="1:13" ht="42" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="107" t="s">
+      <c r="B12" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="105" t="s">
+      <c r="C12" s="98" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="96"/>
@@ -3938,14 +4014,14 @@
       <c r="L12" s="39"/>
       <c r="M12" s="39"/>
     </row>
-    <row r="13" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="105"/>
+      <c r="C13" s="98"/>
       <c r="D13" s="96"/>
       <c r="E13" s="93" t="s">
         <v>95</v>
@@ -3961,14 +4037,14 @@
       <c r="L13" s="39"/>
       <c r="M13" s="39"/>
     </row>
-    <row r="14" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="98" t="s">
         <v>54</v>
       </c>
       <c r="D14" s="96"/>
@@ -3986,14 +4062,14 @@
       <c r="L14" s="39"/>
       <c r="M14" s="39"/>
     </row>
-    <row r="15" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="107" t="s">
+      <c r="B15" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="98" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="96"/>
@@ -4004,21 +4080,21 @@
         <v>95</v>
       </c>
       <c r="G15" s="39"/>
-      <c r="H15" s="102"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
       <c r="L15" s="39"/>
       <c r="M15" s="39"/>
     </row>
-    <row r="16" spans="1:13" ht="46.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="107" t="s">
+      <c r="B16" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="105" t="s">
+      <c r="C16" s="98" t="s">
         <v>61</v>
       </c>
       <c r="D16" s="96"/>
@@ -4036,14 +4112,14 @@
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
     </row>
-    <row r="17" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="98" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="96"/>
@@ -4061,14 +4137,14 @@
       <c r="L17" s="39"/>
       <c r="M17" s="39"/>
     </row>
-    <row r="18" spans="1:13" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="105" t="s">
+      <c r="C18" s="98" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="96"/>
@@ -4086,14 +4162,14 @@
       <c r="L18" s="39"/>
       <c r="M18" s="39"/>
     </row>
-    <row r="19" spans="1:13" ht="46.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="105" t="s">
+      <c r="C19" s="98" t="s">
         <v>71</v>
       </c>
       <c r="D19" s="96"/>
@@ -4111,14 +4187,14 @@
       <c r="L19" s="39"/>
       <c r="M19" s="39"/>
     </row>
-    <row r="20" spans="1:13" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="111" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="105" t="s">
+    <row r="20" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="104" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="98" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="96"/>
@@ -4136,14 +4212,14 @@
       <c r="L20" s="39"/>
       <c r="M20" s="39"/>
     </row>
-    <row r="21" spans="1:13" ht="42.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="107" t="s">
+      <c r="B21" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="105" t="s">
+      <c r="C21" s="98" t="s">
         <v>77</v>
       </c>
       <c r="D21" s="96"/>
@@ -4161,14 +4237,14 @@
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
     </row>
-    <row r="22" spans="1:13" ht="43.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="105" t="s">
+      <c r="C22" s="98" t="s">
         <v>80</v>
       </c>
       <c r="D22" s="96"/>
@@ -4186,14 +4262,14 @@
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
     </row>
-    <row r="23" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="107" t="s">
+      <c r="B23" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="105" t="s">
+      <c r="C23" s="98" t="s">
         <v>83</v>
       </c>
       <c r="D23" s="96"/>
@@ -4211,14 +4287,14 @@
       <c r="L23" s="39"/>
       <c r="M23" s="39"/>
     </row>
-    <row r="24" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="B24" s="107" t="s">
+      <c r="B24" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="105" t="s">
+      <c r="C24" s="98" t="s">
         <v>86</v>
       </c>
       <c r="D24" s="96"/>
@@ -4236,14 +4312,14 @@
       <c r="L24" s="39"/>
       <c r="M24" s="39"/>
     </row>
-    <row r="25" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="105" t="s">
+      <c r="C25" s="98" t="s">
         <v>89</v>
       </c>
       <c r="D25" s="96"/>
@@ -4261,10 +4337,10 @@
       <c r="L25" s="39"/>
       <c r="M25" s="39"/>
     </row>
-    <row r="26" spans="1:13" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:13" ht="45.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="80"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="105"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="96"/>
       <c r="E26" s="93" t="s">
         <v>95</v>
@@ -4280,17 +4356,17 @@
       <c r="L26" s="39"/>
       <c r="M26" s="39"/>
     </row>
-    <row r="27" spans="1:13" ht="26.4" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:13" ht="45.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
       <c r="E27" s="93"/>
       <c r="F27" s="95"/>
     </row>
-    <row r="28" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:13" ht="45.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="E28" s="93"/>
       <c r="F28" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="79" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>